<commit_message>
Added more missing stars
</commit_message>
<xml_diff>
--- a/data-preparation/checklist.xlsx
+++ b/data-preparation/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veronica\Documents\WPI\WPI 2021-22\CS480X\final\data-preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F42F704-1E9E-4EBA-8210-840C024AE172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4CDE0F-7853-4CDB-85E4-65DA334EC444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{540B0EB6-26FA-4CE6-BF3C-386416E49C7A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -306,37 +306,7 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Missing/Error</t>
-  </si>
-  <si>
-    <t>Skewed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missing  </t>
-  </si>
-  <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>Flipped?</t>
-  </si>
-  <si>
-    <t>VZ?</t>
   </si>
 </sst>
 </file>
@@ -690,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DDF3CA-7C61-4E21-82EF-AC7F6FC321DD}">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,15 +677,15 @@
         <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>94</v>
+      <c r="B2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -730,16 +700,16 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>98</v>
+      <c r="B4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>90</v>
+      <c r="B5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -770,8 +740,8 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>90</v>
+      <c r="B9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -786,16 +756,16 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>99</v>
+      <c r="B11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>100</v>
+      <c r="B12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -830,23 +800,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -854,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -862,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -870,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -878,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -886,15 +856,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -902,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -910,15 +880,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -926,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -934,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -942,15 +912,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -958,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -966,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -974,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -982,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -990,15 +957,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1006,23 +970,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="C40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1030,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1038,23 +999,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1062,15 +1020,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1078,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1086,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1094,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1102,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1110,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1118,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1126,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1134,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1142,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1150,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1158,23 +1116,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="C58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1182,15 +1140,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="C61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1198,15 +1153,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1214,15 +1166,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="C65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1230,15 +1182,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1246,15 +1198,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="C69" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1262,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1270,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1278,31 +1227,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="C73" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1310,15 +1256,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="C77" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1326,15 +1272,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="C79" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1342,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1350,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1358,47 +1304,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-      <c r="C83" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-      <c r="C85" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="C86" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="C87" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1406,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>

</xml_diff>